<commit_message>
Adding Adult Education elements
</commit_message>
<xml_diff>
--- a/Data Dictionaries (Upload Here)/SDE/SDE_Data_Dictionary.xlsx
+++ b/Data Dictionaries (Upload Here)/SDE/SDE_Data_Dictionary.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\opm-fs102\UserRedirections\WonderlyC\Documents\Data-Dictionaries\Data Dictionaries (Upload Here)\SDE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ctgovexec-my.sharepoint.com/personal/coral_wonderly_ct_gov/Documents/Open Data/Data-Dictionaries/Data Dictionaries (Upload Here)/SDE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A26CB9-E1F9-4BF5-8D47-ABB9CF41E42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{58A26CB9-E1F9-4BF5-8D47-ABB9CF41E42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB5E72A3-2C34-49A6-9389-4C2852AB6FBA}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="18000" windowHeight="9300" xr2:uid="{824AFC85-3A12-46BD-86EC-A220207FE9A3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{824AFC85-3A12-46BD-86EC-A220207FE9A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$521</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3647" uniqueCount="1077">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4228" uniqueCount="1235">
   <si>
     <t>Agency</t>
   </si>
@@ -3278,6 +3281,747 @@
   </si>
   <si>
     <t>Program</t>
+  </si>
+  <si>
+    <t>Adult Education</t>
+  </si>
+  <si>
+    <t>Unique Individual Identifier (PIRL Element 100)</t>
+  </si>
+  <si>
+    <t>Record the unique identification number assigned to the participant. At a minimum, this identifier for a person must be the same for each program entry and exit (i.e., "period of participation") that an participant has during a program year so that a unique count of participants may be calculated for the program year. NOTE: For Titles I, II, and III, unless specifically directed in program guidance, this field cannot contain a social security number.</t>
+  </si>
+  <si>
+    <t>Unique identification number assigned to the participant.</t>
+  </si>
+  <si>
+    <t>Not Available</t>
+  </si>
+  <si>
+    <t>Date of Birth (PIRL Element 200)</t>
+  </si>
+  <si>
+    <t>Participant's date of birth.</t>
+  </si>
+  <si>
+    <t>YYYYMMDD</t>
+  </si>
+  <si>
+    <t>Sex (PIRL Element 201)</t>
+  </si>
+  <si>
+    <t>1 = Male
+ 2 = Female
+ 9 = Participant did not self-identify</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Individual with a Disability (PIRL Element 202)</t>
+  </si>
+  <si>
+    <t>If the participant indicates that he/she has any "disability”, as defined in Section 3(2)(a) of the Americans with Disabilities Act of 1990 (42 U.S.C. 12102). 
+ 1 = Yes
+ 0 = No
+ 9 = Participant did not self-identify</t>
+  </si>
+  <si>
+    <t>Ethnicity: Hispanic / Latino (PIRL Element 210)</t>
+  </si>
+  <si>
+    <t>1 = Yes
+ 0 = No
+ 9 = Participant did not self-identify</t>
+  </si>
+  <si>
+    <t>American Indian / Alaska Native (PIRL Element 211)</t>
+  </si>
+  <si>
+    <t>Asian (PIRL Element 212)</t>
+  </si>
+  <si>
+    <t>Black / African American (PIRL Element 213)</t>
+  </si>
+  <si>
+    <t>Native Hawaiian / Other Pacific Islander (PIRL Element 214)</t>
+  </si>
+  <si>
+    <t>White (PIRL Element 215)</t>
+  </si>
+  <si>
+    <t>Employment Status at Program Entry (PIRL Element 400)</t>
+  </si>
+  <si>
+    <t>1 = Employed
+ 2 = Employed, but Received Notice of Termination of Employment or Military Separation is pending
+ 3 = Not in labor force
+ 0 = Unemployed</t>
+  </si>
+  <si>
+    <t>Long-Term Unemployed at Program Entry (PIRL Element 402)</t>
+  </si>
+  <si>
+    <t>1 = Yes, Unemployed ≥ 27 consecutive weeks
+ 0 = No</t>
+  </si>
+  <si>
+    <t>Highest School Grade Completed at Program Entry (PIRL Element 407)</t>
+  </si>
+  <si>
+    <t>1 – 12 = Number of school grades completed
+ 0 = No school grades completed</t>
+  </si>
+  <si>
+    <t>School Status at Program Entry (PIRL Element 409)</t>
+  </si>
+  <si>
+    <t>1 = In-school, secondary school or less
+ 2 = In-school, Alternative School
+ 3 = In-school, Postsecondary school.
+ 4 = Not attending school or Secondary School Dropout
+ 5 = Not attending school; secondary school graduate or has a recognized equivalent
+ 6 = Not attending school; within age of compulsory school attendance</t>
+  </si>
+  <si>
+    <t>Exhausting TANF Within 2 Years (PIRL Element 601)</t>
+  </si>
+  <si>
+    <t>If the participant, at program entry, is within 2 years of exhausting lifetime eligibility under part A of Title IV of the Social Security Act (42 U.S.C. 601 et seq.), regardless of whether receiving these benefits at program entry.
+ 1 = Yes
+ 0 = No
+ 9 = Not Applicable</t>
+  </si>
+  <si>
+    <t>Foster Care Youth Status at Program Entry (PIRL Element 704)</t>
+  </si>
+  <si>
+    <t>If the participant, at program entry, is a person aged 24 or under who is currently in foster care or has aged out of the foster care system.
+ 1 = Yes
+ 0 = No</t>
+  </si>
+  <si>
+    <t>Homeless participant, Homeless Children and Youths, or Runaway Youth at Program Entry (PIRL Element 800)</t>
+  </si>
+  <si>
+    <t>If the participant, at program entry:
+ (a) Lacks a fixed, regular, and adequate nighttime residence; this includes a participant who:
+ (i) is sharing the housing of other persons due to loss of housing, economic hardship, or a similar reason;
+ (ii) is living in a motel, hotel, trailer park, or campground due to a lack of alternative adequate accommodations;
+ (iii) is living in an emergency or transitional shelter;
+ (iv) is abandoned in a hospital; or
+ (v) is awaiting foster care placement;
+ (b) Has a primary nighttime residence that is a public or private place not designed for or ordinarily used as a regular sleeping accommodation for human beings, such as a car, park, abandoned building, bus or train station, airport, or camping ground; 
+ (c) Is a migratory child who in the preceding 36 months was required to move from one school district to another due to changes in the parent’s or parent’s spouse’s seasonal employment in agriculture, dairy, or fishing work; or  
+ (d) Is under 18 years of age and absents himself or herself from home or place of legal residence without the permission of his or her family (i.e., runaway youth).
+ 1 = Yes
+ 0 = No</t>
+  </si>
+  <si>
+    <t>Ex-Offender Status at Program Entry
+ (PIRL Element 801)</t>
+  </si>
+  <si>
+    <t>If the participant, at program entry, is a person who either (a) has been subject to any stage of the criminal justice process for committing a status offense or delinquent act, or (b) requires assistance in overcoming barriers to employment resulting from a record of arrest or conviction.
+ 1 = Yes
+ 0 = No
+ 9 = Did not disclose</t>
+  </si>
+  <si>
+    <t>Low Income Status at Program Entry
+  (PIRL Element 802)</t>
+  </si>
+  <si>
+    <t>If the participant, at program entry, is a person who: 
+ (a) Receives, or in the 6 months prior to application to the program has received, or is a member of a family that is receiving or in the past 6 months prior to application to the program has received:
+  (i) Assistance through the supplemental nutrition assistance program (SNAP) under the Food and Nutrition Act of 2008 (7 USC 2011 et seq.);  
+ (ii) Assistance through the temporary assistance for needy families program under part A of Title IV of the Social Security Act (42 USC 601 et seq.);
+ (iii) Assistance through the supplemental security income program under Title XVI of the Social Security Act (42 USC 1381); or
+ (iv) State or local income-based public assistance.
+ (b) Is in a family with total family income that does not exceed the higher of the poverty line or 70% of the lower living standard income level; 
+ (c) Is an individual who receives, or is eligible to receive a free or reduced price lunch under the Richard B. Russell National School Lunch Act (42 USC 1751 et seq.); 
+ (d) Is a foster child on behalf of whom State or local government payments are made;
+ (e) Is an participant with a disability whose own income is the poverty line but who is a member of a family whose income does not meet this requirement;
+ (f) Is a homeless participant or a homeless child or youth or runaway youth (see Data Element 800); or 
+ (g) Is a youth living in a high-poverty area. 
+  1 = Yes
+  0 = No</t>
+  </si>
+  <si>
+    <t>English Language Learner at Program Entry
+ (PIRL Element 803)</t>
+  </si>
+  <si>
+    <t>If the participant, at program entry, is a person who has limited ability in speaking, reading, writing or understanding the English language and also meets at least one of the following two conditions (a) his or her native language is a language other than English, or (b) he or she lives in a family or community environment where a language other than English is the dominant language.
+  1 = Yes
+  0 = No</t>
+  </si>
+  <si>
+    <t>Basic Skills Deficient/Low Levels of Literacy at Program Entry (PIRL Element 804)</t>
+  </si>
+  <si>
+    <t>If the participant is, at program entry:
+ A) a youth, who has English reading, writing, or computing skills at or below the 8th grade level on a generally accepted standardized test; or
+ B) a youth or adult, who is unable to compute and solve problems, or read, write, or speak English at a level necessary to function on the job, in the participant’s family, or in society. 
+  1 = Yes
+  0 = No</t>
+  </si>
+  <si>
+    <t>Cultural Barriers at Program Entry (PIRL Element 805)</t>
+  </si>
+  <si>
+    <t>If the participant, at program entry, perceives him or herself as possessing attitudes, beliefs, customs or practices that influence a way of thinking, acting or working that may serve as a hindrance to employment.
+ 1 = Yes
+ 0 = No                                                                                                                                                                                                                                                                                                                                                                                                                                                                    9 = Participant did not self-identify</t>
+  </si>
+  <si>
+    <t>Single Parent at Program Entry (PIRL Element 806)</t>
+  </si>
+  <si>
+    <t>If the participant, at program entry, is single, separated, divorced or a widowed individual who has primary responsibility for one or more dependent children under age 18 (including single pregnant women).
+ 1 = Yes
+ 0 = No                                                                                                                                                                                                                                                                                                                                                                                                                                                                9 = Participant did not self-identif</t>
+  </si>
+  <si>
+    <t>Displaced Homemaker at Program Entry (PIRL Element 807)</t>
+  </si>
+  <si>
+    <t>If the participant, at program entry, has been providing unpaid services to family members in the home and who:
+         (A)(i) has been dependent on the income of another family member but is no longer supported by that income;  or (ii) is the dependent spouse of a member of the Armed Forces on active duty (as defined in section 101(d)(1) of title 10, United States Code) and whose family income is significantly reduced because of a deployment (as defined in section 991(b) of title 10, United States Code, or pursuant to paragraph (4) of such section), a call or order to active duty pursuant to a provision of law referred to in section 101(a)(13)(B) of title 10, United States Code, a permanent change of station, or the service-connected (as defined in section 101(16) of title 38, United States Code) death or disability of the member; and
+         (B) is unemployed or underemployed and is experiencing difficulty in obtaining or upgrading employment.
+  1 = Yes
+  0 = No</t>
+  </si>
+  <si>
+    <t>Migrant and Seasonal Farmworker Status (PIRL Element 808)</t>
+  </si>
+  <si>
+    <t>1 = Seasonal Farmworker Adult
+ 2 = Migrant Farmworker Adult
+ 3= MSFW Youth
+ 4= Dependent Adult 
+ 5= Dependent Youth 
+ 0 = No</t>
+  </si>
+  <si>
+    <t>Date of Program Entry (PIRL Element 900)</t>
+  </si>
+  <si>
+    <t>The date on which an individual became a participant as referenced in 20 CFR 677.150 satisfying applicable programmatic requirements for the provision of services.</t>
+  </si>
+  <si>
+    <t>Date of Program Exit (PIRL Element 901)</t>
+  </si>
+  <si>
+    <t>The last date the participant received services that are not self-service, information-only, or follow up services.</t>
+  </si>
+  <si>
+    <t>WIOA Adult Participant (PIRL Element 903)</t>
+  </si>
+  <si>
+    <t>1 = Yes, Local Formula
+ 2 = Yes, Statewide
+ 3 = Yes, Both Local Formula and Statewide
+ 4 = Reportable Individual
+ 0 = No</t>
+  </si>
+  <si>
+    <t>WIOA Dislocated Worker Participant (PIRL Element 904)</t>
+  </si>
+  <si>
+    <t>WIOA Youth Participant (PIRL Element 905)</t>
+  </si>
+  <si>
+    <t>Adult Education (PIRL Element 910)</t>
+  </si>
+  <si>
+    <t>if the participant received services under WIOA Title II defined as academic instruction and education services below the postsecondary level that increases an individual’s ability to--- 
+ (A) read, write, and speak in English and perform mathematics or other activities necessary for the attainment of a secondary school diploma or its recognized equivalent;
+ (B) transition to postsecondary education and training; and
+ (C) obtain employment.
+  1 = Yes
+  0 = No
+  9 = Unknown</t>
+  </si>
+  <si>
+    <t>Job Corps (PIRL Element 911)</t>
+  </si>
+  <si>
+    <t>1 if the participant received services under title I, chapter 4, subtitle C of WIOA.
+2 if the individual received reportable individual services (as defined in program specific guidance).
+0 if the individual did not receive any services under the conditions described above.
+9 if grantee is unable to track enrollment in the program.</t>
+  </si>
+  <si>
+    <t>Vocational Rehabilitation (PIRL Element 917)</t>
+  </si>
+  <si>
+    <t>If the participant received services under parts A and B of title I of the Rehabilitation Act of 1973 (29 USC 720 et seq.), WIOA title IV, and Sec. 411(B)(15) defined as transition services for students with disabilities, that facilitate the transition from school to postsecondary life, such as achievement of an employment outcome in competitive integrated employment, or pre-employment transition services. OR
+ If the participant received services from the Vocational Rehabilitation and Employment (VR&amp;E) Program authorized by 38 USC Chapter 31. OR
+ Record 3 if the participant received services from both vocational rehabilitation programs.
+ 1 = Yes
+ 2 = VR&amp;E 
+ 3 = Both VR and VR&amp;E 
+ 0 = No
+ 9 = Unknown</t>
+  </si>
+  <si>
+    <t>Wagner-Peyser Employment Service (PIRL Element 918)</t>
+  </si>
+  <si>
+    <t>If the participant received services under the Wagner-Peyser Act (29 USC 49 et seq.) OR 
+ If the individual has demonstrated an intent to use program services and meets one of the following criteria--- 
+ (A) Individuals who provide identifying information;
+ (B) Individuals who only use the self-service system; or
+ (C) Individuals who only receive information-only services or activities.
+ 1 = Yes
+ 2 = Reportable Individual
+ 0 = No
+ 9 = Unknown</t>
+  </si>
+  <si>
+    <t>YouthBuild (PIRL Element 919)</t>
+  </si>
+  <si>
+    <t>The 14 character grant number if the participant received services under the YouthBuild Program as authorized under WIOA section 171.</t>
+  </si>
+  <si>
+    <t>Other Reasons for Exit (PIRL Element 923)</t>
+  </si>
+  <si>
+    <t>01 = Institutionalized
+ 02 = Health/Medical
+ 03 = Deceased                                                                                                                                                                                                                                                                                                                                                                                                                                                    04 = Reserve Forces called to Active Duty
+ 05 = Foster Care
+ 06 = Ineligible 
+ 07 = Criminal Offender
+ 00 = No</t>
+  </si>
+  <si>
+    <t>Date of Most Recent Career Service (PIRL Element 1004)</t>
+  </si>
+  <si>
+    <t>The date on which career services (both basic and individualized) were last received (excluding self-services, information services or activities, or follow-up services).
+ Blank if the participant did not receive career services.</t>
+  </si>
+  <si>
+    <t>Received Training (PIRL Element 1300)</t>
+  </si>
+  <si>
+    <t>1 = Yes
+ 0 = No</t>
+  </si>
+  <si>
+    <t>Eligible Training Provider - Name - Training Service #1                                                                                                                                                                                                                                  (WIOA)(PIRL Element 1301)</t>
+  </si>
+  <si>
+    <t>Enter the name of the eligible training provider where the participant received training.
+ Leave blank if this data element does not apply to the participant.</t>
+  </si>
+  <si>
+    <t>Date Entered Training #1 (PIRL Element 1302)</t>
+  </si>
+  <si>
+    <t>The date on which the participant's first training service actually began.  
+ Leave blank if the participant did not receive a first training service or this data element does not apply to the participant.</t>
+  </si>
+  <si>
+    <t>Type of Training Service #1 (PIRL Element 1303)</t>
+  </si>
+  <si>
+    <t>4 = On the Job Training (non-WIOA Youth).
+ 02 = Skill Upgrading
+ 03 = Entrepreneurial Training (non-WIOA Youth)
+ 04 = ABE or ESL (contextualized or other) in conjunction with Training
+ 05 = Customized Training
+ 06 = Occupational Skills Training (non-WIOA Youth)
+ 07 = ABE or ESL (contextualized or other) NOT in conjunction with training (funded by Trade Adjustment Assistance only)
+ 08 = Prerequisite Training
+ 09 = Registered Apprenticeship 
+ 10 = Youth Occupational Skills Training                                                                                                            
+ 11 = Other Non-Occupational-Skills Training   
+ 12 = Job Readiness Training in conjunction with other training                                                   
+ 00 = No Training Service                                                                                                                                                                                                                                                                                                                                                                 Leave blank if this data element does not apply to the participant.</t>
+  </si>
+  <si>
+    <t>Eligible Training Provider - Program of Study by Potential Outcome (PIRL Element 1304)</t>
+  </si>
+  <si>
+    <t>1 = A program of study leading to an industry-recognized certificate or certification
+ 2 = A program of study leading to a certificate of completion of a registered apprenticeship
+ 3 = A program of study leading to a license recognized by the State involved or the Federal Government
+ 4 = A program of study leading to an associate degree
+ 5 = A program of study leading to a baccalaureate degree
+ 6 = A program of study leading to a community college certificate of completion
+ 7 = A program of study leading to a secondary school diploma or its equivalent
+ 8 = A program of study leading to employment
+ 9 = A program of study leading to  a measurable skills gain</t>
+  </si>
+  <si>
+    <t>Eligible Training Provider - CIP Code (PIRL Element 1305)</t>
+  </si>
+  <si>
+    <t>This field should represent the 6-digit CIP code, without decimal points.</t>
+  </si>
+  <si>
+    <t>Type of Training Service #2  (PIRL Element 1310)</t>
+  </si>
+  <si>
+    <t>01 = On the Job Training (non-WIOA Youth)
+ 02 = Skill Upgrading
+ 03 = Entrepreneurial Training (non-WIOA Youth)
+ 04 = ABE or ESL (contextualized or other) in conjunction with Training
+ 05 = Customized Training
+ 06 = Occupational Skills Training (non-WIOA Youth)
+ 07 = ABE or ESL (contextualized or other) NOT in conjunction with training (funded by Trade Adjustment Assistance only)
+ 08 = Prerequisite Training
+ 09 = Registered Apprenticeship 
+ 10 = Youth Occupational Skills Training                                                                                                            
+ 11 = Other Non-Occupational-Skills Training   
+ 12 = Job Readiness Training in conjunction with other training                                                   
+ 00 = No Training Service
+ Leave blank if this data element does not apply to the participant.</t>
+  </si>
+  <si>
+    <t>Type of Training Service #3 (PIRL Element 1315)</t>
+  </si>
+  <si>
+    <t>01 = On the Job Training (non-WIOA Youth)
+ 02 = Skill Upgrading
+ 03 = Entrepreneurial Training (non-WIOA Youth)
+ 04 = ABE or ESL (contextualized or other) in conjunction with Training
+ 05 = Customized Training
+ 06 = Occupational Skills Training (non-WIOA Youth)
+ 07 = ABE or ESL (contextualized or other) NOT in conjunction with training (funded by Trade Adjustment Assistance only)
+ 08 = Prerequisite Training
+ 09 = Registered Apprenticeship 
+ 10 = Youth Occupational Skills Training                                                                                                            
+ 11 = Other Non-Occupational-Skills Training   
+ 12 = Job Readiness Training in conjunction with other training                                                   
+ 00 = No Training Service
+ Leave blank if this data element does not apply to the participant.
+ Additional Note: If the participant receives more than three training services, record the last (or most recent) training services received by the participant in this field.</t>
+  </si>
+  <si>
+    <t>Participated in Postsecondary Education During Program Participation (PIRL Element 1332)</t>
+  </si>
+  <si>
+    <t>1 = Yes, Participated in Postsecondary Education  
+ 0 = No, Did Not Participate in Postsecondary Education
+ Leave blank if the participant was not in a postsecondary education program, as defined in program specific guidance.
+ Note: This data element relates to the credential indicator denominator and those who are recorded as 1 are included in the credential rate denominator.  This element is a subset of PIRL 1811.  Do not record 1 if the participant was first enrolled in postsecondary education after exiting the program.</t>
+  </si>
+  <si>
+    <t>Received training from program(s) operated by the private sector (PIRL Element 1333)</t>
+  </si>
+  <si>
+    <t>1 = Yes (received training services from one or more programs operated by the private sector under WIOA sec. 134 (c)(3)(D)(v)). 
+ 0 = No ( did not receive training services from a program operated by the private sector under WIOA sec. 134 (c)(3)(D)(v)).
+ Leave blank if the participant did not receive training.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enrolled in Secondary Education Program (PIRL Element 1401)                                                                                                                                                                                                                                      </t>
+  </si>
+  <si>
+    <t>1 = Yes (participant was enrolled in a Secondary Education Program at or above the 9th Grade level.)
+ 0 = No (participant was not enrolled in a secondary education program at or above the 9th grade level.)</t>
+  </si>
+  <si>
+    <t>Employed in 1st Quarter After Exit Quarter (PIRL Element 1600)</t>
+  </si>
+  <si>
+    <t>1 = Yes (participant is in unsubsidized employment (not including Registered Apprenticeship, or the military). 
+ 2 = Yes, Registered Apprenticeship
+ 3 = Yes, Military 
+ 0 = No (participant was not employed in the first quarter after the quarter of exit.) 
+ 9 = Information not yet available (participant has exited but employment information is not yet available.)</t>
+  </si>
+  <si>
+    <t>Type of Employment Match 1st Quarter After Exit Quarter (PIRL Element 1601)</t>
+  </si>
+  <si>
+    <t>method used in determining the participant's employment status in the first quarter following the quarter of exit. 
+ If the participant is found in more than one source of employment using wage records, record the data source for which the participant's earnings are greatest.
+ 1 = UI Wage Data
+ 2 = Federal Employment Records (OPM, USPS)
+ 3 = Military Employment Records (DOD)
+ 4 = Non UI verification
+ 5 = Information not yet available
+ 0 = Not employed</t>
+  </si>
+  <si>
+    <t>Employed in 2nd Quarter After Exit Quarter (PIRL Element 1602)</t>
+  </si>
+  <si>
+    <t>1 = Yes ( participant is in unsubsidized employment (not including Registered Apprenticeship, or the military).)
+ 2 = Yes, Registered Apprenticeship
+ 3 = Yes, Military
+ 0 = No (participant was not employed in the second quarter after the quarter of exit.)
+ 9 = Information not yet available (participant has exited but employment information is not yet available.)</t>
+  </si>
+  <si>
+    <t>Type of Employment Match 2nd Quarter After Exit Quarter  (PIRL Element 1603)</t>
+  </si>
+  <si>
+    <t>1 = UI Wage Data 
+ 2 = Federal Employment Records (OPM, USPS)
+ 3 = Military Employment Records (DOD)
+ 4 = Non UI verification                                      
+ 5 = Information not yet available
+ 0 = Not employed</t>
+  </si>
+  <si>
+    <t>Employed in 3rd Quarter After Exit Quarter (PIRL Element 1604)</t>
+  </si>
+  <si>
+    <t>1 = Yes (participant is in unsubsidized employment (not including Registered Apprenticeship, or the military).) 
+ 2 = Yes, Registered Apprenticeship
+ 3 = Yes, Military                                                     
+ 0 = No ( participant was not employed in the third quarter after the quarter of exit.) 
+ 9 = Information not yet available ( (participant has exited but employment information is not yet available.) )</t>
+  </si>
+  <si>
+    <t>Type of Employment Match 3rd Quarter After Exit Quarter (PIRL Element 1605)</t>
+  </si>
+  <si>
+    <t>1 = UI Wage Data
+ 2 = Federal Employment Records (OPM, USPS)
+ 3 = Military Employment Records (DOD)
+ 4 = Non UI verification 
+ 5 = Information not yet available
+ 0 = Not employed</t>
+  </si>
+  <si>
+    <t>Employed in 4th Quarter After Exit Quarter (PIRL Element 1606)</t>
+  </si>
+  <si>
+    <t>1 = Yes ( participant is in unsubsidized employment (not including Registered Apprenticeship, or the military).) 
+ 2 = Yes, Registered Apprenticeship
+ 3 = Yes, Military 
+  0 = No (participant was not employed in the fourth quarter after the quarter of exit.) 
+ 9 = Information not yet available</t>
+  </si>
+  <si>
+    <t>Type of Employment Match 4th Quarter After Exit Quarter (PIRL Element 1607)</t>
+  </si>
+  <si>
+    <t>1 = UI Wage Data 
+ 2 = Federal Employment Records (OPM, USPS)
+ 3 = Military Employment Records (DOD)
+ 4 = Non UI verification 
+ 5 = Information not yet available
+ 0 = Not employed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employment Related to Training (2nd Quarter After Exit) (PIRL Element 1608)                                                                                                                                                                                                                                                                                                                                                                                                           </t>
+  </si>
+  <si>
+    <t>1 = Training related to employment
+ 0 = Training not related to employment
+ 9 = Unknown
+ Leave blank if the participant did not receive training or has not exited or the employment information is not yet available.</t>
+  </si>
+  <si>
+    <t>Retention with the same employer in the 2nd Quarter and the 4th Quarter (PIRL Element 1618)</t>
+  </si>
+  <si>
+    <t>1 = Yes (the participant’s employer in the second quarter also matches the employer in the fourth quarter)    
+ 0 = No ( the participant is not employed in the second or fourth quarters after exit, or the employer in the second quarter does not match the employer in the fourth quarter)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Earnings 1st Quarter After Exit Quarter (PIRL Element 1703)                                                                                                                                                                                                                                                                                                                                                                                            </t>
+  </si>
+  <si>
+    <t>Total earnings for the first quarter after the quarter of exit.
+ Record 9999999.99 if data is are not yet available for this item.
+ Leave blank if data element does not apply to the participant.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Earnings 2nd Quarter After Exit Quarter (PIRL Element 1704)                                                                                                                                                                                                                                                                                                                                                                                                   </t>
+  </si>
+  <si>
+    <t>Total earnings for the second quarter after the quarter of exit.
+ Record 9999999.99 if data is not yet available for this item.
+ Leave blank if data element does not apply to the participant.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Earnings 3rd Quarter After Exit Quarter (PIRL Element 1705)                                                                                                                                                                                                                                                                                                                                                                                                  </t>
+  </si>
+  <si>
+    <t>Total earnings for the third quarter after the quarter of exit.
+ Record 9999999.99 if data is not yet available for this item.
+ Leave blank if data element does not apply to the participant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Earnings 4th Quarter After Exit Quarter (PIRL Element 1706)                                                                                                                                                                                                                                                                                                                                                               </t>
+  </si>
+  <si>
+    <t>total earnings for the fourth quarter after the quarter of exit.
+ Record 9999999.99 if data is not yet available for this item.
+ Leave blank if data element does not apply to the participant.</t>
+  </si>
+  <si>
+    <t>Type of Recognized Credential (PIRL Element 1800)</t>
+  </si>
+  <si>
+    <t>Diplomas, degrees, licenses or certificates must be attained either during participation or within one year of exit. This data element applies to both the Credential Rate indicator and the Measurable Skills Gain indicator  for all programs. 
+ 1 = Secondary School Diploma/or equivalency 
+ 2 = AA or AS Diploma/Degree
+ 3 = BA or BS Diploma/Degree
+ 4 = Occupational Licensure
+ 5 = Occupational Certificate
+ 6 = Occupational Certification
+ 7 = Other Recognized Diploma, Degree, or Certificate
+ 0 = No recognized credential
+ Leave blank if data element does not apply to the participant.</t>
+  </si>
+  <si>
+    <t>Date Attained Recognized Credential (PIRL Element 1801)</t>
+  </si>
+  <si>
+    <t>The date on which the participant attained a recognized credential. 
+ Leave blank if the participant did not attain a degree or certificate.</t>
+  </si>
+  <si>
+    <t>Type of Recognized Credential #2 (PIRL Element 1802)</t>
+  </si>
+  <si>
+    <t>Diplomas, degrees, licenses or certificates must be attained either during participation or within one year of exit. This data element applies to both the Credential Rate indicator and the Measurable Skills Gain indicator for all DOL programs. 
+ 1 = Secondary School Diploma/or equivalency 
+ 2 = AA or AS Diploma/Degree
+ 3 = BA or BS Diploma/Degree
+ 4 = Occupational Licensure
+ 5 = Occupational Certificate
+ 6 = Occupational Certification
+ 7 = Other Recognized Diploma, Degree, or Certificate
+ 0 = No recognized credential
+ Leave blank if data element does not apply to the participant.</t>
+  </si>
+  <si>
+    <t>Date Attained Recognized Credential #2 (PIRL Element 1803)</t>
+  </si>
+  <si>
+    <t>The date on which the participant attained a second recognized credential.  
+ Leave blank if the participant did not attain a second recognized credential, or if this data element does not apply.</t>
+  </si>
+  <si>
+    <t>Type of Recognized Credential #3 (PIRL Element 1804)</t>
+  </si>
+  <si>
+    <t>Diplomas, degrees, licenses or certificates must be attained either during participation or within one year of exit. This data element applies to both the Credential Rate indicator and the Measurable Skills Gain indicator for all DOL programs.
+ 1 = Secondary School Diploma/or equivalency 
+ 2 = AA or AS Diploma/Degree
+ 3 = BA or BS Diploma/Degree
+ 4 = Occupational Licensure
+ 5 = Occupational Certificate
+ 6 = Occupational Certification
+ 7 = Other Recognized Diploma, Degree, or Certificate
+ 0 = No recognized credential
+ Leave blank if data element does not apply to the participant.</t>
+  </si>
+  <si>
+    <t>Date Attained Recognized Credential #3 (PIRL Element 1805)</t>
+  </si>
+  <si>
+    <t>The date on which the participant attained a third recognized credential.  
+ Leave blank if the participant did not attain a third recognized credential, or if this data element does not apply.</t>
+  </si>
+  <si>
+    <t>Date of Most Recent Measurable Skill Gains: Educational Functioning Level (EFL) (PIRL Element 1806)</t>
+  </si>
+  <si>
+    <t>The most recent date the participant who received instruction below the postsecondary education level achieved at least one EFL.  
+ EFL  gain may be documented in one of three ways: 
+ 1) by comparing a participant’s  initial EFL as measured by a pre-test with the participant’s EFL as measured by a participant’s post-test; or 
+ 2) for States that offer secondary school programs that lead to a secondary school diploma or its recognized equivalent, an EFL gain may be measured through the awarding of credits or Carnegie units: or 3) States may report an EFL gain for participants who exit the program and enroll in postsecondary education or training during the program year. 
+ Leave blank if this data element does not apply to the participant.</t>
+  </si>
+  <si>
+    <t>Date of Most Recent Measurable Skill Gains: Postsecondary Transcript/Report Card (PIRL Element 1807)</t>
+  </si>
+  <si>
+    <t>The most recent date of the participant’s transcript or report card for postsecondary education who complete a minimum of 12 hours per semester, or for part time students a total of at least 12 credit hours over the course of two completed semesters during the same 12 month period, that shows a participant is meeting the State unit's academic standards. 
+ Leave blank if this data element does not apply to the participant.</t>
+  </si>
+  <si>
+    <t>Date of Most Recent Measurable Skill Gains: Secondary Transcript/Report Card (PIRL Element 1808)</t>
+  </si>
+  <si>
+    <t>The most recent date of the participant’s transcript or report card for secondary education for one semester showing that the participant is meeting the State unit’s academic standards. 
+ Leave blank if this data element does not apply to the participant.</t>
+  </si>
+  <si>
+    <t>Date of Most Recent Measurable Skill Gains: Training Milestone (PIRL Element 1809)</t>
+  </si>
+  <si>
+    <t>The most recent date that the participant had a satisfactory or better progress report towards established milestones from an employer/training provider who is providing training (e.g., completion of on-the-job training (OJT), completion of one year of a registered apprenticeship program, etc.).               
+ Leave blank if this data element does not apply to the participant.</t>
+  </si>
+  <si>
+    <t>Date of Most Recent Measurable Skill Gains: Skills Progression (PIRL Element 1810)</t>
+  </si>
+  <si>
+    <t>The most recent date the participant successfully completed an exam that is required for a particular occupation, or progress in attaining technical or occupational skills as evidenced by trade-related benchmarks such as knowledge-based exams.
+ Leave blank if this data element does not apply to the participant.</t>
+  </si>
+  <si>
+    <t>Date Enrolled During Program Participation in an Education or Training Program Leading to a Recognized Credential or Employment (PIRL Element 1811)</t>
+  </si>
+  <si>
+    <t>The date the participant was enrolled during program participation in an education or training program that either 
+ 1) leads to a recognized  credential, including a secondary education program; or 
+ 2) a training program that leads to employment; as defined by the core program in which the participant participates.
+ If the participant was enrolled in postsecondary education at program entry, the date in this field should be the date of Program Entry. This includes, but is not limited to, participation in Job Corps, YouthBuild, a Registered Apprenticeship program, Adult Education or secondary education programs.
+ Leave blank if the  data element does not apply to the participant.    
+                                                                                                                                                                                                                                                                                                                                                                                                                                                                        NOTE: This data element applies to the Measurable Skill Gains Indicator, and specifically will be utilized to calculate the denominator. It encompasses all education and training program enrollment.</t>
+  </si>
+  <si>
+    <t>Date Completed During Program Participation an Education or Training Program Leading to a Recognized Credential or Employment (PIRL Element 1813)</t>
+  </si>
+  <si>
+    <t>The date the participant completes, during program participation, either 
+ 1) an education or training program that leads to a recognized  credential, including a secondary education program; or 
+ 2) training program that leads to employment; as defined by the core program in which the participant participates.
+ Leave blank if the  data element does not apply to the participant.    
+                                                                                                                                                                                                                                                                                                                                                                                                                                                                        NOTE: This data element applies to the Measurable Skill Gains Indicator, and specifically will be utilized to calculate the denominator. It encompasses all education and training program enrollment.</t>
+  </si>
+  <si>
+    <t>Date Attained Graduate/Post Graduate Degree (PIRL Element 1814)</t>
+  </si>
+  <si>
+    <t>The date a participant attained a masters’ degree after receiving education or training service.
+ Leave blank if data element does not apply to the participant.
+ Diplomas, degrees, licenses or certificates must be attained either during participation or within one year of exit. This data element applies to the Credential Rate for RSA programs.</t>
+  </si>
+  <si>
+    <t>Youth 2nd Quarter Placement (Title I) (PIRL Element 1900)</t>
+  </si>
+  <si>
+    <t>1 = enrolled in Occupational Skills Training (including advanced training).
+ 2 = enrolled in Postsecondary Education
+ 3 = enrolled in Secondary Education
+ 0 = No placement</t>
+  </si>
+  <si>
+    <t>Youth 4th Quarter Placement (Title I) (PIRL Element 1901)</t>
+  </si>
+  <si>
+    <t>1 =  enrolled in Occupational Skills Training (including advanced training).
+ 2 = enrolled in Postsecondary Education
+ 3 = enrolled in Secondary Education
+ 0 = No placement</t>
+  </si>
+  <si>
+    <t>Incarcerated at Program Entry (PIRL Element 2413)</t>
+  </si>
+  <si>
+    <t>Date Released from Incarceration (PIRL Element 2414)</t>
+  </si>
+  <si>
+    <t>Date the participant was released from a correctional institution.</t>
+  </si>
+  <si>
+    <t>If the participant was a criminal offender in a correctional institution at program entry.</t>
   </si>
 </sst>
 </file>
@@ -3638,21 +4382,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{655E8F63-11E4-41F5-A5D0-443FBAFD2251}">
-  <dimension ref="A1:G521"/>
+  <dimension ref="A1:G604"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D556" sqref="D556:G556"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.42578125" customWidth="1"/>
-    <col min="5" max="5" width="33" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" customWidth="1"/>
-    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="66.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -9689,7 +10433,7 @@
         <v>15</v>
       </c>
       <c r="C263" t="s">
-        <v>565</v>
+        <v>1077</v>
       </c>
       <c r="D263" t="s">
         <v>566</v>
@@ -9712,7 +10456,7 @@
         <v>15</v>
       </c>
       <c r="C264" t="s">
-        <v>565</v>
+        <v>1077</v>
       </c>
       <c r="D264" t="s">
         <v>568</v>
@@ -9735,7 +10479,7 @@
         <v>15</v>
       </c>
       <c r="C265" t="s">
-        <v>565</v>
+        <v>1077</v>
       </c>
       <c r="D265" t="s">
         <v>570</v>
@@ -15636,6 +16380,1915 @@
       </c>
       <c r="G521" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="522" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A522" t="s">
+        <v>14</v>
+      </c>
+      <c r="B522" t="s">
+        <v>15</v>
+      </c>
+      <c r="C522" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D522" t="s">
+        <v>1078</v>
+      </c>
+      <c r="E522" t="s">
+        <v>1079</v>
+      </c>
+      <c r="F522" t="s">
+        <v>1045</v>
+      </c>
+      <c r="G522" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="523" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A523" t="s">
+        <v>14</v>
+      </c>
+      <c r="B523" t="s">
+        <v>15</v>
+      </c>
+      <c r="C523" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D523" t="s">
+        <v>1078</v>
+      </c>
+      <c r="E523" t="s">
+        <v>1080</v>
+      </c>
+      <c r="F523" t="s">
+        <v>91</v>
+      </c>
+      <c r="G523" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="524" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A524" t="s">
+        <v>14</v>
+      </c>
+      <c r="B524" t="s">
+        <v>15</v>
+      </c>
+      <c r="C524" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D524" t="s">
+        <v>1082</v>
+      </c>
+      <c r="E524" t="s">
+        <v>1083</v>
+      </c>
+      <c r="F524" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G524" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="525" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A525" t="s">
+        <v>14</v>
+      </c>
+      <c r="B525" t="s">
+        <v>15</v>
+      </c>
+      <c r="C525" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D525" t="s">
+        <v>1085</v>
+      </c>
+      <c r="E525" t="s">
+        <v>1086</v>
+      </c>
+      <c r="F525" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G525" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="526" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A526" t="s">
+        <v>14</v>
+      </c>
+      <c r="B526" t="s">
+        <v>15</v>
+      </c>
+      <c r="C526" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D526" t="s">
+        <v>1088</v>
+      </c>
+      <c r="E526" t="s">
+        <v>1089</v>
+      </c>
+      <c r="F526" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G526" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="527" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A527" t="s">
+        <v>14</v>
+      </c>
+      <c r="B527" t="s">
+        <v>15</v>
+      </c>
+      <c r="C527" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D527" t="s">
+        <v>1090</v>
+      </c>
+      <c r="E527" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F527" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G527" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="528" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A528" t="s">
+        <v>14</v>
+      </c>
+      <c r="B528" t="s">
+        <v>15</v>
+      </c>
+      <c r="C528" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D528" t="s">
+        <v>1092</v>
+      </c>
+      <c r="E528" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F528" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G528" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="529" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A529" t="s">
+        <v>14</v>
+      </c>
+      <c r="B529" t="s">
+        <v>15</v>
+      </c>
+      <c r="C529" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D529" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E529" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F529" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G529" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="530" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A530" t="s">
+        <v>14</v>
+      </c>
+      <c r="B530" t="s">
+        <v>15</v>
+      </c>
+      <c r="C530" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D530" t="s">
+        <v>1094</v>
+      </c>
+      <c r="E530" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F530" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G530" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="531" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A531" t="s">
+        <v>14</v>
+      </c>
+      <c r="B531" t="s">
+        <v>15</v>
+      </c>
+      <c r="C531" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D531" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E531" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F531" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G531" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="532" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A532" t="s">
+        <v>14</v>
+      </c>
+      <c r="B532" t="s">
+        <v>15</v>
+      </c>
+      <c r="C532" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D532" t="s">
+        <v>1096</v>
+      </c>
+      <c r="E532" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F532" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G532" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="533" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A533" t="s">
+        <v>14</v>
+      </c>
+      <c r="B533" t="s">
+        <v>15</v>
+      </c>
+      <c r="C533" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D533" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E533" t="s">
+        <v>1098</v>
+      </c>
+      <c r="F533" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G533" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="534" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A534" t="s">
+        <v>14</v>
+      </c>
+      <c r="B534" t="s">
+        <v>15</v>
+      </c>
+      <c r="C534" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D534" t="s">
+        <v>1099</v>
+      </c>
+      <c r="E534" t="s">
+        <v>1100</v>
+      </c>
+      <c r="F534" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G534" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="535" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A535" t="s">
+        <v>14</v>
+      </c>
+      <c r="B535" t="s">
+        <v>15</v>
+      </c>
+      <c r="C535" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D535" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E535" t="s">
+        <v>1102</v>
+      </c>
+      <c r="F535" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G535" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="536" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A536" t="s">
+        <v>14</v>
+      </c>
+      <c r="B536" t="s">
+        <v>15</v>
+      </c>
+      <c r="C536" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D536" t="s">
+        <v>1103</v>
+      </c>
+      <c r="E536" t="s">
+        <v>1104</v>
+      </c>
+      <c r="F536" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G536" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="537" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A537" t="s">
+        <v>14</v>
+      </c>
+      <c r="B537" t="s">
+        <v>15</v>
+      </c>
+      <c r="C537" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D537" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E537" t="s">
+        <v>1102</v>
+      </c>
+      <c r="F537" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G537" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="538" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A538" t="s">
+        <v>14</v>
+      </c>
+      <c r="B538" t="s">
+        <v>15</v>
+      </c>
+      <c r="C538" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D538" t="s">
+        <v>1103</v>
+      </c>
+      <c r="E538" t="s">
+        <v>1104</v>
+      </c>
+      <c r="F538" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G538" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="539" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A539" t="s">
+        <v>14</v>
+      </c>
+      <c r="B539" t="s">
+        <v>15</v>
+      </c>
+      <c r="C539" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D539" t="s">
+        <v>1105</v>
+      </c>
+      <c r="E539" t="s">
+        <v>1106</v>
+      </c>
+      <c r="F539" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G539" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="540" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A540" t="s">
+        <v>14</v>
+      </c>
+      <c r="B540" t="s">
+        <v>15</v>
+      </c>
+      <c r="C540" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D540" t="s">
+        <v>1107</v>
+      </c>
+      <c r="E540" t="s">
+        <v>1108</v>
+      </c>
+      <c r="F540" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G540" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="541" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A541" t="s">
+        <v>14</v>
+      </c>
+      <c r="B541" t="s">
+        <v>15</v>
+      </c>
+      <c r="C541" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D541" t="s">
+        <v>1109</v>
+      </c>
+      <c r="E541" t="s">
+        <v>1110</v>
+      </c>
+      <c r="F541" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G541" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="542" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A542" t="s">
+        <v>14</v>
+      </c>
+      <c r="B542" t="s">
+        <v>15</v>
+      </c>
+      <c r="C542" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D542" t="s">
+        <v>1111</v>
+      </c>
+      <c r="E542" t="s">
+        <v>1112</v>
+      </c>
+      <c r="F542" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G542" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="543" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A543" t="s">
+        <v>14</v>
+      </c>
+      <c r="B543" t="s">
+        <v>15</v>
+      </c>
+      <c r="C543" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D543" t="s">
+        <v>1113</v>
+      </c>
+      <c r="E543" t="s">
+        <v>1114</v>
+      </c>
+      <c r="F543" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G543" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="544" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A544" t="s">
+        <v>14</v>
+      </c>
+      <c r="B544" t="s">
+        <v>15</v>
+      </c>
+      <c r="C544" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D544" t="s">
+        <v>1115</v>
+      </c>
+      <c r="E544" t="s">
+        <v>1116</v>
+      </c>
+      <c r="F544" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G544" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="545" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A545" t="s">
+        <v>14</v>
+      </c>
+      <c r="B545" t="s">
+        <v>15</v>
+      </c>
+      <c r="C545" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D545" t="s">
+        <v>1117</v>
+      </c>
+      <c r="E545" t="s">
+        <v>1118</v>
+      </c>
+      <c r="F545" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G545" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="546" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A546" t="s">
+        <v>14</v>
+      </c>
+      <c r="B546" t="s">
+        <v>15</v>
+      </c>
+      <c r="C546" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D546" t="s">
+        <v>1119</v>
+      </c>
+      <c r="E546" t="s">
+        <v>1120</v>
+      </c>
+      <c r="F546" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G546" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="547" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A547" t="s">
+        <v>14</v>
+      </c>
+      <c r="B547" t="s">
+        <v>15</v>
+      </c>
+      <c r="C547" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D547" t="s">
+        <v>1121</v>
+      </c>
+      <c r="E547" t="s">
+        <v>1122</v>
+      </c>
+      <c r="F547" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G547" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="548" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A548" t="s">
+        <v>14</v>
+      </c>
+      <c r="B548" t="s">
+        <v>15</v>
+      </c>
+      <c r="C548" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D548" t="s">
+        <v>1123</v>
+      </c>
+      <c r="E548" t="s">
+        <v>1124</v>
+      </c>
+      <c r="F548" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G548" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="549" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A549" t="s">
+        <v>14</v>
+      </c>
+      <c r="B549" t="s">
+        <v>15</v>
+      </c>
+      <c r="C549" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D549" t="s">
+        <v>1125</v>
+      </c>
+      <c r="E549" t="s">
+        <v>1126</v>
+      </c>
+      <c r="F549" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G549" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="550" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A550" t="s">
+        <v>14</v>
+      </c>
+      <c r="B550" t="s">
+        <v>15</v>
+      </c>
+      <c r="C550" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D550" t="s">
+        <v>1127</v>
+      </c>
+      <c r="E550" t="s">
+        <v>1128</v>
+      </c>
+      <c r="F550" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G550" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="551" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A551" t="s">
+        <v>14</v>
+      </c>
+      <c r="B551" t="s">
+        <v>15</v>
+      </c>
+      <c r="C551" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D551" t="s">
+        <v>1129</v>
+      </c>
+      <c r="E551" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F551" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G551" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="552" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A552" t="s">
+        <v>14</v>
+      </c>
+      <c r="B552" t="s">
+        <v>15</v>
+      </c>
+      <c r="C552" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D552" t="s">
+        <v>1131</v>
+      </c>
+      <c r="E552" t="s">
+        <v>1132</v>
+      </c>
+      <c r="F552" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G552" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="553" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A553" t="s">
+        <v>14</v>
+      </c>
+      <c r="B553" t="s">
+        <v>15</v>
+      </c>
+      <c r="C553" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D553" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E553" t="s">
+        <v>1132</v>
+      </c>
+      <c r="F553" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G553" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="554" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A554" t="s">
+        <v>14</v>
+      </c>
+      <c r="B554" t="s">
+        <v>15</v>
+      </c>
+      <c r="C554" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D554" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E554" t="s">
+        <v>1132</v>
+      </c>
+      <c r="F554" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G554" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="555" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A555" t="s">
+        <v>14</v>
+      </c>
+      <c r="B555" t="s">
+        <v>15</v>
+      </c>
+      <c r="C555" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D555" t="s">
+        <v>1135</v>
+      </c>
+      <c r="E555" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F555" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G555" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="556" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A556" t="s">
+        <v>14</v>
+      </c>
+      <c r="B556" t="s">
+        <v>15</v>
+      </c>
+      <c r="C556" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D556" t="s">
+        <v>1137</v>
+      </c>
+      <c r="E556" t="s">
+        <v>1138</v>
+      </c>
+      <c r="F556" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G556" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="557" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A557" t="s">
+        <v>14</v>
+      </c>
+      <c r="B557" t="s">
+        <v>15</v>
+      </c>
+      <c r="C557" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D557" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E557" t="s">
+        <v>1140</v>
+      </c>
+      <c r="F557" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G557" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="558" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A558" t="s">
+        <v>14</v>
+      </c>
+      <c r="B558" t="s">
+        <v>15</v>
+      </c>
+      <c r="C558" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D558" t="s">
+        <v>1141</v>
+      </c>
+      <c r="E558" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F558" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G558" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="559" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A559" t="s">
+        <v>14</v>
+      </c>
+      <c r="B559" t="s">
+        <v>15</v>
+      </c>
+      <c r="C559" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D559" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E559" t="s">
+        <v>1144</v>
+      </c>
+      <c r="F559" t="s">
+        <v>91</v>
+      </c>
+      <c r="G559" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="560" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A560" t="s">
+        <v>14</v>
+      </c>
+      <c r="B560" t="s">
+        <v>15</v>
+      </c>
+      <c r="C560" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D560" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E560" t="s">
+        <v>1146</v>
+      </c>
+      <c r="F560" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G560" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="561" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A561" t="s">
+        <v>14</v>
+      </c>
+      <c r="B561" t="s">
+        <v>15</v>
+      </c>
+      <c r="C561" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D561" t="s">
+        <v>1147</v>
+      </c>
+      <c r="E561" t="s">
+        <v>1148</v>
+      </c>
+      <c r="F561" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G561" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="562" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A562" t="s">
+        <v>14</v>
+      </c>
+      <c r="B562" t="s">
+        <v>15</v>
+      </c>
+      <c r="C562" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D562" t="s">
+        <v>1149</v>
+      </c>
+      <c r="E562" t="s">
+        <v>1150</v>
+      </c>
+      <c r="F562" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G562" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="563" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A563" t="s">
+        <v>14</v>
+      </c>
+      <c r="B563" t="s">
+        <v>15</v>
+      </c>
+      <c r="C563" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D563" t="s">
+        <v>1151</v>
+      </c>
+      <c r="E563" t="s">
+        <v>1152</v>
+      </c>
+      <c r="F563" t="s">
+        <v>1081</v>
+      </c>
+      <c r="G563" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="564" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A564" t="s">
+        <v>14</v>
+      </c>
+      <c r="B564" t="s">
+        <v>15</v>
+      </c>
+      <c r="C564" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D564" t="s">
+        <v>1153</v>
+      </c>
+      <c r="E564" t="s">
+        <v>1154</v>
+      </c>
+      <c r="F564" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G564" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="565" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A565" t="s">
+        <v>14</v>
+      </c>
+      <c r="B565" t="s">
+        <v>15</v>
+      </c>
+      <c r="C565" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D565" t="s">
+        <v>1155</v>
+      </c>
+      <c r="E565" t="s">
+        <v>1156</v>
+      </c>
+      <c r="F565" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G565" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="566" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A566" t="s">
+        <v>14</v>
+      </c>
+      <c r="B566" t="s">
+        <v>15</v>
+      </c>
+      <c r="C566" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D566" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E566" t="s">
+        <v>1158</v>
+      </c>
+      <c r="F566" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G566" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="567" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A567" t="s">
+        <v>14</v>
+      </c>
+      <c r="B567" t="s">
+        <v>15</v>
+      </c>
+      <c r="C567" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D567" t="s">
+        <v>1159</v>
+      </c>
+      <c r="E567" t="s">
+        <v>1160</v>
+      </c>
+      <c r="F567" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G567" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="568" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A568" t="s">
+        <v>14</v>
+      </c>
+      <c r="B568" t="s">
+        <v>15</v>
+      </c>
+      <c r="C568" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D568" t="s">
+        <v>1161</v>
+      </c>
+      <c r="E568" t="s">
+        <v>1162</v>
+      </c>
+      <c r="F568" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G568" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="569" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A569" t="s">
+        <v>14</v>
+      </c>
+      <c r="B569" t="s">
+        <v>15</v>
+      </c>
+      <c r="C569" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D569" t="s">
+        <v>1163</v>
+      </c>
+      <c r="E569" t="s">
+        <v>1164</v>
+      </c>
+      <c r="F569" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G569" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="570" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A570" t="s">
+        <v>14</v>
+      </c>
+      <c r="B570" t="s">
+        <v>15</v>
+      </c>
+      <c r="C570" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D570" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E570" t="s">
+        <v>1166</v>
+      </c>
+      <c r="F570" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G570" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="571" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A571" t="s">
+        <v>14</v>
+      </c>
+      <c r="B571" t="s">
+        <v>15</v>
+      </c>
+      <c r="C571" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D571" t="s">
+        <v>1167</v>
+      </c>
+      <c r="E571" t="s">
+        <v>1168</v>
+      </c>
+      <c r="F571" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G571" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="572" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A572" t="s">
+        <v>14</v>
+      </c>
+      <c r="B572" t="s">
+        <v>15</v>
+      </c>
+      <c r="C572" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D572" t="s">
+        <v>1169</v>
+      </c>
+      <c r="E572" t="s">
+        <v>1170</v>
+      </c>
+      <c r="F572" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G572" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="573" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A573" t="s">
+        <v>14</v>
+      </c>
+      <c r="B573" t="s">
+        <v>15</v>
+      </c>
+      <c r="C573" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D573" t="s">
+        <v>1171</v>
+      </c>
+      <c r="E573" t="s">
+        <v>1172</v>
+      </c>
+      <c r="F573" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G573" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="574" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A574" t="s">
+        <v>14</v>
+      </c>
+      <c r="B574" t="s">
+        <v>15</v>
+      </c>
+      <c r="C574" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D574" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E574" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F574" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G574" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="575" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A575" t="s">
+        <v>14</v>
+      </c>
+      <c r="B575" t="s">
+        <v>15</v>
+      </c>
+      <c r="C575" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D575" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E575" t="s">
+        <v>1176</v>
+      </c>
+      <c r="F575" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G575" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="576" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A576" t="s">
+        <v>14</v>
+      </c>
+      <c r="B576" t="s">
+        <v>15</v>
+      </c>
+      <c r="C576" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D576" t="s">
+        <v>1177</v>
+      </c>
+      <c r="E576" t="s">
+        <v>1178</v>
+      </c>
+      <c r="F576" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G576" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="577" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A577" t="s">
+        <v>14</v>
+      </c>
+      <c r="B577" t="s">
+        <v>15</v>
+      </c>
+      <c r="C577" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D577" t="s">
+        <v>1179</v>
+      </c>
+      <c r="E577" t="s">
+        <v>1180</v>
+      </c>
+      <c r="F577" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G577" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="578" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A578" t="s">
+        <v>14</v>
+      </c>
+      <c r="B578" t="s">
+        <v>15</v>
+      </c>
+      <c r="C578" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D578" t="s">
+        <v>1181</v>
+      </c>
+      <c r="E578" t="s">
+        <v>1182</v>
+      </c>
+      <c r="F578" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G578" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="579" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A579" t="s">
+        <v>14</v>
+      </c>
+      <c r="B579" t="s">
+        <v>15</v>
+      </c>
+      <c r="C579" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D579" t="s">
+        <v>1183</v>
+      </c>
+      <c r="E579" t="s">
+        <v>1184</v>
+      </c>
+      <c r="F579" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G579" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="580" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A580" t="s">
+        <v>14</v>
+      </c>
+      <c r="B580" t="s">
+        <v>15</v>
+      </c>
+      <c r="C580" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D580" t="s">
+        <v>1185</v>
+      </c>
+      <c r="E580" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F580" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G580" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="581" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A581" t="s">
+        <v>14</v>
+      </c>
+      <c r="B581" t="s">
+        <v>15</v>
+      </c>
+      <c r="C581" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D581" t="s">
+        <v>1187</v>
+      </c>
+      <c r="E581" t="s">
+        <v>1188</v>
+      </c>
+      <c r="F581" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G581" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="582" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A582" t="s">
+        <v>14</v>
+      </c>
+      <c r="B582" t="s">
+        <v>15</v>
+      </c>
+      <c r="C582" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D582" t="s">
+        <v>1189</v>
+      </c>
+      <c r="E582" t="s">
+        <v>1190</v>
+      </c>
+      <c r="F582" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G582" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="583" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A583" t="s">
+        <v>14</v>
+      </c>
+      <c r="B583" t="s">
+        <v>15</v>
+      </c>
+      <c r="C583" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D583" t="s">
+        <v>1191</v>
+      </c>
+      <c r="E583" t="s">
+        <v>1192</v>
+      </c>
+      <c r="F583" t="s">
+        <v>91</v>
+      </c>
+      <c r="G583" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="584" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A584" t="s">
+        <v>14</v>
+      </c>
+      <c r="B584" t="s">
+        <v>15</v>
+      </c>
+      <c r="C584" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D584" t="s">
+        <v>1193</v>
+      </c>
+      <c r="E584" t="s">
+        <v>1194</v>
+      </c>
+      <c r="F584" t="s">
+        <v>91</v>
+      </c>
+      <c r="G584" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="585" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A585" t="s">
+        <v>14</v>
+      </c>
+      <c r="B585" t="s">
+        <v>15</v>
+      </c>
+      <c r="C585" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D585" t="s">
+        <v>1195</v>
+      </c>
+      <c r="E585" t="s">
+        <v>1196</v>
+      </c>
+      <c r="F585" t="s">
+        <v>91</v>
+      </c>
+      <c r="G585" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="586" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A586" t="s">
+        <v>14</v>
+      </c>
+      <c r="B586" t="s">
+        <v>15</v>
+      </c>
+      <c r="C586" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D586" t="s">
+        <v>1197</v>
+      </c>
+      <c r="E586" t="s">
+        <v>1198</v>
+      </c>
+      <c r="F586" t="s">
+        <v>91</v>
+      </c>
+      <c r="G586" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="587" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A587" t="s">
+        <v>14</v>
+      </c>
+      <c r="B587" t="s">
+        <v>15</v>
+      </c>
+      <c r="C587" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D587" t="s">
+        <v>1199</v>
+      </c>
+      <c r="E587" t="s">
+        <v>1200</v>
+      </c>
+      <c r="F587" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G587" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="588" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A588" t="s">
+        <v>14</v>
+      </c>
+      <c r="B588" t="s">
+        <v>15</v>
+      </c>
+      <c r="C588" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D588" t="s">
+        <v>1201</v>
+      </c>
+      <c r="E588" t="s">
+        <v>1202</v>
+      </c>
+      <c r="F588" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G588" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="589" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A589" t="s">
+        <v>14</v>
+      </c>
+      <c r="B589" t="s">
+        <v>15</v>
+      </c>
+      <c r="C589" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D589" t="s">
+        <v>1203</v>
+      </c>
+      <c r="E589" t="s">
+        <v>1204</v>
+      </c>
+      <c r="F589" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G589" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="590" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A590" t="s">
+        <v>14</v>
+      </c>
+      <c r="B590" t="s">
+        <v>15</v>
+      </c>
+      <c r="C590" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D590" t="s">
+        <v>1205</v>
+      </c>
+      <c r="E590" t="s">
+        <v>1206</v>
+      </c>
+      <c r="F590" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G590" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="591" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A591" t="s">
+        <v>14</v>
+      </c>
+      <c r="B591" t="s">
+        <v>15</v>
+      </c>
+      <c r="C591" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D591" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E591" t="s">
+        <v>1208</v>
+      </c>
+      <c r="F591" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G591" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="592" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A592" t="s">
+        <v>14</v>
+      </c>
+      <c r="B592" t="s">
+        <v>15</v>
+      </c>
+      <c r="C592" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D592" t="s">
+        <v>1209</v>
+      </c>
+      <c r="E592" t="s">
+        <v>1210</v>
+      </c>
+      <c r="F592" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G592" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="593" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A593" t="s">
+        <v>14</v>
+      </c>
+      <c r="B593" t="s">
+        <v>15</v>
+      </c>
+      <c r="C593" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D593" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E593" t="s">
+        <v>1212</v>
+      </c>
+      <c r="F593" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G593" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="594" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A594" t="s">
+        <v>14</v>
+      </c>
+      <c r="B594" t="s">
+        <v>15</v>
+      </c>
+      <c r="C594" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D594" t="s">
+        <v>1213</v>
+      </c>
+      <c r="E594" t="s">
+        <v>1214</v>
+      </c>
+      <c r="F594" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G594" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="595" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A595" t="s">
+        <v>14</v>
+      </c>
+      <c r="B595" t="s">
+        <v>15</v>
+      </c>
+      <c r="C595" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D595" t="s">
+        <v>1215</v>
+      </c>
+      <c r="E595" t="s">
+        <v>1216</v>
+      </c>
+      <c r="F595" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G595" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="596" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A596" t="s">
+        <v>14</v>
+      </c>
+      <c r="B596" t="s">
+        <v>15</v>
+      </c>
+      <c r="C596" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D596" t="s">
+        <v>1217</v>
+      </c>
+      <c r="E596" t="s">
+        <v>1218</v>
+      </c>
+      <c r="F596" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G596" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="597" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A597" t="s">
+        <v>14</v>
+      </c>
+      <c r="B597" t="s">
+        <v>15</v>
+      </c>
+      <c r="C597" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D597" t="s">
+        <v>1219</v>
+      </c>
+      <c r="E597" t="s">
+        <v>1220</v>
+      </c>
+      <c r="F597" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G597" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="598" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A598" t="s">
+        <v>14</v>
+      </c>
+      <c r="B598" t="s">
+        <v>15</v>
+      </c>
+      <c r="C598" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D598" t="s">
+        <v>1221</v>
+      </c>
+      <c r="E598" t="s">
+        <v>1222</v>
+      </c>
+      <c r="F598" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G598" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="599" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A599" t="s">
+        <v>14</v>
+      </c>
+      <c r="B599" t="s">
+        <v>15</v>
+      </c>
+      <c r="C599" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D599" t="s">
+        <v>1223</v>
+      </c>
+      <c r="E599" t="s">
+        <v>1224</v>
+      </c>
+      <c r="F599" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G599" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="600" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A600" t="s">
+        <v>14</v>
+      </c>
+      <c r="B600" t="s">
+        <v>15</v>
+      </c>
+      <c r="C600" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D600" t="s">
+        <v>1225</v>
+      </c>
+      <c r="E600" t="s">
+        <v>1226</v>
+      </c>
+      <c r="F600" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G600" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="601" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A601" t="s">
+        <v>14</v>
+      </c>
+      <c r="B601" t="s">
+        <v>15</v>
+      </c>
+      <c r="C601" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D601" t="s">
+        <v>1227</v>
+      </c>
+      <c r="E601" t="s">
+        <v>1228</v>
+      </c>
+      <c r="F601" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G601" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="602" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A602" t="s">
+        <v>14</v>
+      </c>
+      <c r="B602" t="s">
+        <v>15</v>
+      </c>
+      <c r="C602" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D602" t="s">
+        <v>1229</v>
+      </c>
+      <c r="E602" t="s">
+        <v>1230</v>
+      </c>
+      <c r="F602" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G602" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="603" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A603" t="s">
+        <v>14</v>
+      </c>
+      <c r="B603" t="s">
+        <v>15</v>
+      </c>
+      <c r="C603" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D603" t="s">
+        <v>1232</v>
+      </c>
+      <c r="E603" t="s">
+        <v>1234</v>
+      </c>
+      <c r="F603" t="s">
+        <v>47</v>
+      </c>
+      <c r="G603" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="604" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A604" t="s">
+        <v>14</v>
+      </c>
+      <c r="B604" t="s">
+        <v>15</v>
+      </c>
+      <c r="C604" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D604" t="s">
+        <v>1231</v>
+      </c>
+      <c r="E604" t="s">
+        <v>1233</v>
+      </c>
+      <c r="F604" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G604" t="s">
+        <v>1081</v>
       </c>
     </row>
   </sheetData>

</xml_diff>